<commit_message>
partial updates fr new version.
</commit_message>
<xml_diff>
--- a/excelfiles/Core_Vocabularies_v1.2.xlsx
+++ b/excelfiles/Core_Vocabularies_v1.2.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8820" tabRatio="522" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8820" tabRatio="522" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="CoreVocabularies" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,23 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TargetVocabulary!$B$1:$L$587</definedName>
     <definedName name="_xlcn.WorksheetConnection_Core_Vocabularies_template.xlsxCoreVocabularies1" hidden="1">CoreVocabularies[]</definedName>
     <definedName name="_xlcn.WorksheetConnection_Core_Vocabularies_template.xlsxRelations1" hidden="1">Relations[]</definedName>
-    <definedName name="Address">CoreVocabularies!$B$2</definedName>
-    <definedName name="AddressAddressArea">CoreVocabularies!$B$8</definedName>
-    <definedName name="AddressAddressID">CoreVocabularies!$B$13</definedName>
-    <definedName name="AddressAdminUnitL1">CoreVocabularies!$B$11</definedName>
-    <definedName name="AddressAdminUnitL2">CoreVocabularies!$B$10</definedName>
-    <definedName name="AddressFullAddress">CoreVocabularies!$B$3</definedName>
-    <definedName name="AddressLocatorDesignator">CoreVocabularies!$B$6</definedName>
-    <definedName name="AddressLocatorName">CoreVocabularies!$B$7</definedName>
-    <definedName name="AddressPOBox">CoreVocabularies!$B$4</definedName>
-    <definedName name="AddressPostCode">CoreVocabularies!$B$12</definedName>
-    <definedName name="AddressPostName">CoreVocabularies!$B$9</definedName>
-    <definedName name="AddressThoroughfare">CoreVocabularies!$B$5</definedName>
-    <definedName name="Agent">CoreVocabularies!$B$14</definedName>
-    <definedName name="AgentPlaysRole">CoreVocabularies!$B$15</definedName>
-    <definedName name="AgentProvides">CoreVocabularies!$B$16</definedName>
-    <definedName name="AgentUses">CoreVocabularies!$B$17</definedName>
-    <definedName name="Channel">CoreVocabularies!$B$18</definedName>
+    <definedName name="Address">'CoreVocabularies'!$B$2</definedName>
+    <definedName name="AddressAddressArea">'CoreVocabularies'!$B$8</definedName>
+    <definedName name="AddressAddressID">'CoreVocabularies'!$B$13</definedName>
+    <definedName name="AddressAdminUnitL1">'CoreVocabularies'!$B$11</definedName>
+    <definedName name="AddressAdminUnitL2">'CoreVocabularies'!$B$10</definedName>
+    <definedName name="AddressFullAddress">'CoreVocabularies'!$B$3</definedName>
+    <definedName name="AddressLocatorDesignator">'CoreVocabularies'!$B$6</definedName>
+    <definedName name="AddressLocatorName">'CoreVocabularies'!$B$7</definedName>
+    <definedName name="AddressPOBox">'CoreVocabularies'!$B$4</definedName>
+    <definedName name="AddressPostCode">'CoreVocabularies'!$B$12</definedName>
+    <definedName name="AddressPostName">'CoreVocabularies'!$B$9</definedName>
+    <definedName name="AddressThoroughfare">'CoreVocabularies'!$B$5</definedName>
+    <definedName name="Agent">'CoreVocabularies'!$B$14</definedName>
+    <definedName name="AgentPlaysRole">'CoreVocabularies'!$B$15</definedName>
+    <definedName name="AgentProvides">'CoreVocabularies'!$B$16</definedName>
+    <definedName name="AgentUses">'CoreVocabularies'!$B$17</definedName>
+    <definedName name="Channel">'CoreVocabularies'!$B$18</definedName>
     <definedName name="Code">'Data Types'!$A$2</definedName>
     <definedName name="CodeContent">'Data Types'!$A$3</definedName>
     <definedName name="CodeList">'Data Types'!$A$4</definedName>
@@ -128,7 +128,7 @@
     <definedName name="TextLanguage">'Data Types'!$A$18</definedName>
     <definedName name="URI">'Data Types'!$A$19</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId8"/>
   </pivotCaches>
@@ -441,7 +441,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7553" uniqueCount="1614">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7555" uniqueCount="1615">
   <si>
     <t>Term</t>
   </si>
@@ -5281,9 +5281,6 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>Term / Label</t>
-  </si>
-  <si>
     <t>Term/Label</t>
   </si>
   <si>
@@ -5342,6 +5339,12 @@
   </si>
   <si>
     <t>an explanation or comment on the mapping</t>
+  </si>
+  <si>
+    <t>Data model</t>
+  </si>
+  <si>
+    <t>Target Identifier</t>
   </si>
 </sst>
 </file>
@@ -5909,32 +5912,6 @@
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="112">
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -6531,27 +6508,6 @@
       </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="6" tint="0.39994506668294322"/>
@@ -6568,30 +6524,6 @@
           <bgColor theme="6" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -6620,6 +6552,77 @@
           <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -18337,7 +18340,7 @@
     <dataField name="Count of Core Vocabulary Identifier" fld="0" subtotal="count" showDataAs="percentOfRow" baseField="0" baseItem="0" numFmtId="9"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="1">
+    <format dxfId="92">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -18351,41 +18354,41 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="CoreVocabularies" displayName="CoreVocabularies" ref="B1:K89" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="CoreVocabularies" displayName="CoreVocabularies" ref="B1:K89" totalsRowShown="0" headerRowDxfId="111" dataDxfId="110">
   <autoFilter ref="B1:K89"/>
   <tableColumns count="10">
-    <tableColumn id="2" name="Identifier (internal)" dataDxfId="105" dataCellStyle="Normal">
+    <tableColumn id="2" name="Identifier (internal)" dataDxfId="109" dataCellStyle="Normal">
       <calculatedColumnFormula>SUBSTITUTE($E2," ","")&amp;IF($D2&lt;&gt;"Class",SUBSTITUTE($C2," ",""),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" name="Term / Label" dataCellStyle="Normal"/>
+    <tableColumn id="1" name="Term/Label" dataCellStyle="Normal"/>
     <tableColumn id="3" name="Type" dataCellStyle="Normal"/>
     <tableColumn id="4" name="Class" dataCellStyle="Normal"/>
     <tableColumn id="5" name="Data Type" dataCellStyle="Normal"/>
-    <tableColumn id="7" name="Definition" dataDxfId="104" dataCellStyle="Normal"/>
-    <tableColumn id="8" name="Description" dataDxfId="103" dataCellStyle="Normal"/>
-    <tableColumn id="10" name="Public Identifier (URI)" dataDxfId="102"/>
-    <tableColumn id="9" name="Examples" dataDxfId="101" dataCellStyle="Normal"/>
-    <tableColumn id="6" name="Comments for next version" dataDxfId="100" dataCellStyle="Normal"/>
+    <tableColumn id="7" name="Definition" dataDxfId="108" dataCellStyle="Normal"/>
+    <tableColumn id="8" name="Description" dataDxfId="107" dataCellStyle="Normal"/>
+    <tableColumn id="10" name="Public Identifier (URI)" dataDxfId="106"/>
+    <tableColumn id="9" name="Examples" dataDxfId="105" dataCellStyle="Normal"/>
+    <tableColumn id="6" name="Comments for next version" dataDxfId="104" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="DataTypes" displayName="DataTypes" ref="A1:I19" totalsRowShown="0" headerRowDxfId="97" dataDxfId="96">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="DataTypes" displayName="DataTypes" ref="A1:I19" totalsRowShown="0" headerRowDxfId="103" dataDxfId="102">
   <autoFilter ref="A1:I19"/>
   <tableColumns count="9">
-    <tableColumn id="2" name="Identifier" dataDxfId="95" dataCellStyle="Normal">
+    <tableColumn id="2" name="Identifier" dataDxfId="101" dataCellStyle="Normal">
       <calculatedColumnFormula>SUBSTITUTE($D2," ","")&amp;IF($C2="Attribute",SUBSTITUTE($B2," ",""),"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="1" name="Term" dataCellStyle="Normal"/>
     <tableColumn id="3" name="Type" dataCellStyle="Normal"/>
     <tableColumn id="4" name="Data Type" dataCellStyle="Normal"/>
     <tableColumn id="5" name="Primitive Type" dataCellStyle="Normal"/>
-    <tableColumn id="7" name="Definition" dataDxfId="94" dataCellStyle="Normal"/>
-    <tableColumn id="8" name="Description" dataDxfId="93" dataCellStyle="Normal"/>
-    <tableColumn id="9" name="Examples" dataDxfId="92" dataCellStyle="Normal"/>
-    <tableColumn id="6" name="Comments for next version" dataDxfId="91" dataCellStyle="Normal"/>
+    <tableColumn id="7" name="Definition" dataDxfId="100" dataCellStyle="Normal"/>
+    <tableColumn id="8" name="Description" dataDxfId="99" dataCellStyle="Normal"/>
+    <tableColumn id="9" name="Examples" dataDxfId="98" dataCellStyle="Normal"/>
+    <tableColumn id="6" name="Comments for next version" dataDxfId="97" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -18396,15 +18399,15 @@
   <autoFilter ref="A1:H1154"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Core Vocabulary Identifier"/>
-    <tableColumn id="6" name="Link" dataDxfId="5">
+    <tableColumn id="6" name="Link" dataDxfId="96">
       <calculatedColumnFormula>HYPERLINK("#"&amp;$A2,"Link")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" name="Mapping relation"/>
     <tableColumn id="4" name="Data model "/>
-    <tableColumn id="3" name="Identifier" dataDxfId="4"/>
+    <tableColumn id="3" name="Identifier" dataDxfId="95"/>
     <tableColumn id="8" name="Label"/>
-    <tableColumn id="9" name="Definition" dataDxfId="3"/>
-    <tableColumn id="5" name="Mapping comment" dataDxfId="2"/>
+    <tableColumn id="9" name="Definition" dataDxfId="94"/>
+    <tableColumn id="5" name="Mapping comment" dataDxfId="93"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -18415,7 +18418,7 @@
   <autoFilter ref="A1:B9"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Concept"/>
-    <tableColumn id="2" name="Definition" dataDxfId="0"/>
+    <tableColumn id="2" name="Definition" dataDxfId="91"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -18714,15 +18717,15 @@
   <dimension ref="A1:K89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="33.5703125" customWidth="1"/>
     <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
@@ -19251,7 +19254,7 @@
         <v>1591</v>
       </c>
       <c r="B19" t="str">
-        <f t="shared" si="0"/>
+        <f>SUBSTITUTE($E19," ","")&amp;IF($D19&lt;&gt;"Class",SUBSTITUTE($C19," ",""),"")</f>
         <v>FormalFramework</v>
       </c>
       <c r="C19" t="s">
@@ -21211,18 +21214,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:K89">
-    <cfRule type="expression" dxfId="111" priority="3">
+    <cfRule type="expression" dxfId="90" priority="3">
       <formula>$D2 = "Association"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="110" priority="4">
+    <cfRule type="expression" dxfId="89" priority="4">
       <formula>$D2 = "Class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A89">
-    <cfRule type="expression" dxfId="109" priority="1">
+    <cfRule type="expression" dxfId="88" priority="1">
       <formula>$D2 = "Association"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="108" priority="2">
+    <cfRule type="expression" dxfId="87" priority="2">
       <formula>$D2 = "Class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21322,7 +21325,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -21770,10 +21773,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:I19">
-    <cfRule type="expression" dxfId="99" priority="1">
+    <cfRule type="expression" dxfId="86" priority="1">
       <formula>$C2 = "Primitive Type"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="2">
+    <cfRule type="expression" dxfId="85" priority="2">
       <formula>$C2 = "Composite Type"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21812,20 +21815,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L579"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.85546875" customWidth="1"/>
-    <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" customWidth="1"/>
+    <col min="3" max="3" width="35.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.85546875" customWidth="1"/>
+    <col min="8" max="8" width="28.28515625" customWidth="1"/>
     <col min="9" max="9" width="28.140625" customWidth="1"/>
     <col min="10" max="10" width="27.140625" customWidth="1"/>
     <col min="11" max="11" width="9.42578125" customWidth="1"/>
@@ -21834,7 +21837,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="69" t="s">
-        <v>1595</v>
+        <v>1594</v>
       </c>
       <c r="B1" s="69" t="s">
         <v>1590</v>
@@ -21843,7 +21846,7 @@
         <v>1589</v>
       </c>
       <c r="D1" s="69" t="s">
-        <v>1594</v>
+        <v>1593</v>
       </c>
       <c r="E1" s="69" t="s">
         <v>2</v>
@@ -21883,6 +21886,9 @@
       </c>
       <c r="D2" t="s">
         <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
       </c>
       <c r="H2" t="s">
         <v>914</v>
@@ -30716,18 +30722,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="1" max="1" width="43.42578125" customWidth="1"/>
     <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.140625" customWidth="1"/>
-    <col min="5" max="5" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="66.5703125" customWidth="1"/>
+    <col min="5" max="5" width="32.7109375" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" customWidth="1"/>
     <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="34.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="67.42578125" bestFit="1" customWidth="1"/>
@@ -30735,7 +30741,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
-        <v>1598</v>
+        <v>1597</v>
       </c>
       <c r="B1" s="32" t="s">
         <v>1</v>
@@ -30744,19 +30750,19 @@
         <v>862</v>
       </c>
       <c r="D1" s="31" t="s">
-        <v>1596</v>
+        <v>1595</v>
       </c>
       <c r="E1" s="31" t="s">
-        <v>860</v>
+        <v>1613</v>
       </c>
       <c r="F1" s="34" t="s">
-        <v>1</v>
+        <v>1614</v>
       </c>
       <c r="G1" s="52" t="s">
         <v>863</v>
       </c>
       <c r="K1" s="70" t="s">
-        <v>1600</v>
+        <v>1599</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -30768,29 +30774,14 @@
         <f>CoreVocabularies!C2</f>
         <v>Address</v>
       </c>
-      <c r="C2" t="s">
+      <c r="K2" s="32" t="s">
         <v>1597</v>
       </c>
-      <c r="D2" t="str">
-        <f>TargetVocabulary!A2</f>
-        <v>OASIS UBL Common Library 2.1 / Address. Details</v>
-      </c>
-      <c r="E2" t="str">
-        <f>TargetVocabulary!B2</f>
-        <v>OASIS UBL Common Library 2.1</v>
-      </c>
-      <c r="F2" t="str">
-        <f>TargetVocabulary!C2</f>
-        <v>Address. Details</v>
-      </c>
-      <c r="K2" s="32" t="s">
+      <c r="L2" s="32" t="s">
         <v>1598</v>
       </c>
-      <c r="L2" s="32" t="s">
-        <v>1599</v>
-      </c>
       <c r="M2" t="s">
-        <v>1602</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -30802,14 +30793,29 @@
         <f>CoreVocabularies!C3</f>
         <v>Full Address</v>
       </c>
+      <c r="C3" t="s">
+        <v>1596</v>
+      </c>
+      <c r="D3" t="str">
+        <f>TargetVocabulary!A2</f>
+        <v>OASIS UBL Common Library 2.1 / Address. Details</v>
+      </c>
+      <c r="E3" t="str">
+        <f>TargetVocabulary!B2</f>
+        <v>OASIS UBL Common Library 2.1</v>
+      </c>
+      <c r="F3" t="str">
+        <f>TargetVocabulary!C2</f>
+        <v>Address. Details</v>
+      </c>
       <c r="K3" s="32" t="s">
         <v>1</v>
       </c>
       <c r="L3" t="s">
-        <v>1601</v>
+        <v>1600</v>
       </c>
       <c r="M3" t="s">
-        <v>1603</v>
+        <v>1602</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -30825,7 +30831,7 @@
         <v>862</v>
       </c>
       <c r="L4" s="52" t="s">
-        <v>1604</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -30838,13 +30844,13 @@
         <v>Thoroughfare</v>
       </c>
       <c r="K5" s="31" t="s">
+        <v>1604</v>
+      </c>
+      <c r="L5" s="31" t="s">
         <v>1605</v>
       </c>
-      <c r="L5" s="31" t="s">
+      <c r="M5" t="s">
         <v>1606</v>
-      </c>
-      <c r="M5" t="s">
-        <v>1607</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -30857,13 +30863,13 @@
         <v>Locator Designator</v>
       </c>
       <c r="K6" s="31" t="s">
+        <v>1607</v>
+      </c>
+      <c r="L6" s="31" t="s">
         <v>1608</v>
       </c>
-      <c r="L6" s="31" t="s">
-        <v>1609</v>
-      </c>
       <c r="M6" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -30879,10 +30885,10 @@
         <v>1</v>
       </c>
       <c r="L7" s="31" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="M7" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -30898,7 +30904,7 @@
         <v>863</v>
       </c>
       <c r="L8" s="52" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -30939,6 +30945,21 @@
       <c r="B12" t="str">
         <f>CoreVocabularies!C12</f>
         <v>Post Code</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1596</v>
+      </c>
+      <c r="D12" t="str">
+        <f>TargetVocabulary!A15</f>
+        <v>OASIS UBL Common Library 2.1 / Address. Postal_ Zone. Text</v>
+      </c>
+      <c r="E12" t="str">
+        <f>TargetVocabulary!B15</f>
+        <v>OASIS UBL Common Library 2.1</v>
+      </c>
+      <c r="F12" t="str">
+        <f>TargetVocabulary!C15</f>
+        <v>Address. Postal_ Zone. Text</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -31722,7 +31743,7 @@
   <sheetPr codeName="Sheet3" filterMode="1"/>
   <dimension ref="A1:I1154"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -55638,299 +55659,299 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I2:I20 A2:H720 A723:H729 A721:G722 A730:G840">
-    <cfRule type="expression" dxfId="90" priority="141">
+    <cfRule type="expression" dxfId="84" priority="141">
       <formula>$C2 = $I$2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="142">
+    <cfRule type="expression" dxfId="83" priority="142">
       <formula>$C2 = $I$6</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="143">
+    <cfRule type="expression" dxfId="82" priority="143">
       <formula>$C2 = $I$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="87" priority="144">
+    <cfRule type="expression" dxfId="81" priority="144">
       <formula>$C2 = $I$4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="145">
+    <cfRule type="expression" dxfId="80" priority="145">
       <formula>$C2 = $I$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21:I840">
-    <cfRule type="expression" dxfId="85" priority="136">
+    <cfRule type="expression" dxfId="79" priority="136">
       <formula>$C21 = $I$2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="137">
+    <cfRule type="expression" dxfId="78" priority="137">
       <formula>$C21 = $I$6</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="138">
+    <cfRule type="expression" dxfId="77" priority="138">
       <formula>$C21 = $I$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="139">
+    <cfRule type="expression" dxfId="76" priority="139">
       <formula>$C21 = $I$4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="140">
+    <cfRule type="expression" dxfId="75" priority="140">
       <formula>$C21 = $I$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H721:H722">
-    <cfRule type="expression" dxfId="80" priority="131">
+    <cfRule type="expression" dxfId="74" priority="131">
       <formula>$C721 = $I$2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="132">
+    <cfRule type="expression" dxfId="73" priority="132">
       <formula>$C721 = $I$6</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="133">
+    <cfRule type="expression" dxfId="72" priority="133">
       <formula>$C721 = $I$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="77" priority="134">
+    <cfRule type="expression" dxfId="71" priority="134">
       <formula>$C721 = $I$4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="135">
+    <cfRule type="expression" dxfId="70" priority="135">
       <formula>$C721 = $I$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H731:H831">
-    <cfRule type="expression" dxfId="75" priority="125">
+    <cfRule type="expression" dxfId="69" priority="125">
       <formula>$C731 = "Exact match"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H731:H831">
-    <cfRule type="expression" dxfId="74" priority="121">
+    <cfRule type="expression" dxfId="68" priority="121">
       <formula>$C731 = "Related match"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="122">
+    <cfRule type="expression" dxfId="67" priority="122">
       <formula>$C731 = "Narrow match"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="123">
+    <cfRule type="expression" dxfId="66" priority="123">
       <formula>$C731 = "Broad match"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="124">
+    <cfRule type="expression" dxfId="65" priority="124">
       <formula>$C731 = "Close match"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H730">
-    <cfRule type="expression" dxfId="70" priority="120">
+    <cfRule type="expression" dxfId="64" priority="120">
       <formula>$C730 = "Exact match"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H730">
-    <cfRule type="expression" dxfId="69" priority="116">
+    <cfRule type="expression" dxfId="63" priority="116">
       <formula>$C730 = "Related match"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="117">
+    <cfRule type="expression" dxfId="62" priority="117">
       <formula>$C730 = "Narrow match"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="118">
+    <cfRule type="expression" dxfId="61" priority="118">
       <formula>$C730 = "Broad match"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="119">
+    <cfRule type="expression" dxfId="60" priority="119">
       <formula>$C730 = "Close match"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H833:H840">
-    <cfRule type="expression" dxfId="65" priority="115">
+    <cfRule type="expression" dxfId="59" priority="115">
       <formula>$C833 = "Exact match"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H833:H840">
-    <cfRule type="expression" dxfId="64" priority="111">
+    <cfRule type="expression" dxfId="58" priority="111">
       <formula>$C833 = "Related match"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="112">
+    <cfRule type="expression" dxfId="57" priority="112">
       <formula>$C833 = "Narrow match"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="113">
+    <cfRule type="expression" dxfId="56" priority="113">
       <formula>$C833 = "Broad match"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="114">
+    <cfRule type="expression" dxfId="55" priority="114">
       <formula>$C833 = "Close match"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H730:H840">
-    <cfRule type="expression" dxfId="60" priority="126">
+    <cfRule type="expression" dxfId="54" priority="126">
       <formula>$C730 = $K$2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="127">
+    <cfRule type="expression" dxfId="53" priority="127">
       <formula>$C730 = $K$6</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="128">
+    <cfRule type="expression" dxfId="52" priority="128">
       <formula>$C730 = $K$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="129">
+    <cfRule type="expression" dxfId="51" priority="129">
       <formula>$C730 = $K$4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="130">
+    <cfRule type="expression" dxfId="50" priority="130">
       <formula>$C730 = $K$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A841:G841">
-    <cfRule type="expression" dxfId="55" priority="96">
+    <cfRule type="expression" dxfId="49" priority="96">
       <formula>$C841 = $I$2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="97">
+    <cfRule type="expression" dxfId="48" priority="97">
       <formula>$C841 = $I$6</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="98">
+    <cfRule type="expression" dxfId="47" priority="98">
       <formula>$C841 = $I$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="99">
+    <cfRule type="expression" dxfId="46" priority="99">
       <formula>$C841 = $I$4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="100">
+    <cfRule type="expression" dxfId="45" priority="100">
       <formula>$C841 = $I$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I841">
-    <cfRule type="expression" dxfId="50" priority="91">
+    <cfRule type="expression" dxfId="44" priority="91">
       <formula>$C841 = $I$2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="92">
+    <cfRule type="expression" dxfId="43" priority="92">
       <formula>$C841 = $I$6</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="93">
+    <cfRule type="expression" dxfId="42" priority="93">
       <formula>$C841 = $I$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="94">
+    <cfRule type="expression" dxfId="41" priority="94">
       <formula>$C841 = $I$4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="95">
+    <cfRule type="expression" dxfId="40" priority="95">
       <formula>$C841 = $I$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H841">
-    <cfRule type="expression" dxfId="45" priority="85">
+    <cfRule type="expression" dxfId="39" priority="85">
       <formula>$C841 = "Exact match"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H841">
-    <cfRule type="expression" dxfId="44" priority="81">
+    <cfRule type="expression" dxfId="38" priority="81">
       <formula>$C841 = "Related match"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="82">
+    <cfRule type="expression" dxfId="37" priority="82">
       <formula>$C841 = "Narrow match"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="83">
+    <cfRule type="expression" dxfId="36" priority="83">
       <formula>$C841 = "Broad match"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="84">
+    <cfRule type="expression" dxfId="35" priority="84">
       <formula>$C841 = "Close match"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H841">
-    <cfRule type="expression" dxfId="40" priority="86">
+    <cfRule type="expression" dxfId="34" priority="86">
       <formula>$C841 = $K$2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="87">
+    <cfRule type="expression" dxfId="33" priority="87">
       <formula>$C841 = $K$6</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="88">
+    <cfRule type="expression" dxfId="32" priority="88">
       <formula>$C841 = $K$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="89">
+    <cfRule type="expression" dxfId="31" priority="89">
       <formula>$C841 = $K$4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="90">
+    <cfRule type="expression" dxfId="30" priority="90">
       <formula>$C841 = $K$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B842:H842 A842:A953 E844:H849 F843:H843 B843:C914 B915:B929 D843:D953 E851:H929 F850:H850 C915:C953 C1016:C1023 C1025:C1030 C1035:C1036 C1038:C1040 C1042:C1067 C1069:C1070 C1084:C1090 C1106:C1154">
-    <cfRule type="expression" dxfId="35" priority="71">
+    <cfRule type="expression" dxfId="29" priority="71">
       <formula>$C842 = $J$2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="72">
+    <cfRule type="expression" dxfId="28" priority="72">
       <formula>$C842 = $J$6</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="73">
+    <cfRule type="expression" dxfId="27" priority="73">
       <formula>$C842 = $J$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="74">
+    <cfRule type="expression" dxfId="26" priority="74">
       <formula>$C842 = $J$4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="75">
+    <cfRule type="expression" dxfId="25" priority="75">
       <formula>$C842 = $J$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E850">
-    <cfRule type="expression" dxfId="30" priority="76">
+    <cfRule type="expression" dxfId="24" priority="76">
       <formula>$C843 = $J$2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="77">
+    <cfRule type="expression" dxfId="23" priority="77">
       <formula>$C843 = $J$6</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="78">
+    <cfRule type="expression" dxfId="22" priority="78">
       <formula>$C843 = $J$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="79">
+    <cfRule type="expression" dxfId="21" priority="79">
       <formula>$C843 = $J$4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="80">
+    <cfRule type="expression" dxfId="20" priority="80">
       <formula>$C843 = $J$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C954:C956">
-    <cfRule type="expression" dxfId="25" priority="66">
+    <cfRule type="expression" dxfId="19" priority="66">
       <formula>$C954 = $J$2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="67">
+    <cfRule type="expression" dxfId="18" priority="67">
       <formula>$C954 = $J$6</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="68">
+    <cfRule type="expression" dxfId="17" priority="68">
       <formula>$C954 = $J$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="69">
+    <cfRule type="expression" dxfId="16" priority="69">
       <formula>$C954 = $J$4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="70">
+    <cfRule type="expression" dxfId="15" priority="70">
       <formula>$C954 = $J$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C959:C964">
-    <cfRule type="expression" dxfId="20" priority="61">
+    <cfRule type="expression" dxfId="14" priority="61">
       <formula>$C959 = $J$2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="62">
+    <cfRule type="expression" dxfId="13" priority="62">
       <formula>$C959 = $J$6</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="63">
+    <cfRule type="expression" dxfId="12" priority="63">
       <formula>$C959 = $J$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="64">
+    <cfRule type="expression" dxfId="11" priority="64">
       <formula>$C959 = $J$4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="65">
+    <cfRule type="expression" dxfId="10" priority="65">
       <formula>$C959 = $J$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C970:C982">
-    <cfRule type="expression" dxfId="15" priority="56">
+    <cfRule type="expression" dxfId="9" priority="56">
       <formula>$C970 = $J$2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="57">
+    <cfRule type="expression" dxfId="8" priority="57">
       <formula>$C970 = $J$6</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="58">
+    <cfRule type="expression" dxfId="7" priority="58">
       <formula>$C970 = $J$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="59">
+    <cfRule type="expression" dxfId="6" priority="59">
       <formula>$C970 = $J$4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="60">
+    <cfRule type="expression" dxfId="5" priority="60">
       <formula>$C970 = $J$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C983:C1000">
-    <cfRule type="expression" dxfId="10" priority="51">
+    <cfRule type="expression" dxfId="4" priority="51">
       <formula>$C983 = $J$2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="52">
+    <cfRule type="expression" dxfId="3" priority="52">
       <formula>$C983 = $J$6</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="53">
+    <cfRule type="expression" dxfId="2" priority="53">
       <formula>$C983 = $J$5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="54">
+    <cfRule type="expression" dxfId="1" priority="54">
       <formula>$C983 = $J$4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="55">
+    <cfRule type="expression" dxfId="0" priority="55">
       <formula>$C983 = $J$3</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>